<commit_message>
Última versión del proyecto
</commit_message>
<xml_diff>
--- a/explicaciones.xlsx
+++ b/explicaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaba\Documents\Ciencia_de_Datos\Ciencia_Datos_IV\Practicas_Externas\Proyecto_Shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA0B4B3-E73A-4CBE-A3C8-8DA7C56F13A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792C34A5-2BA0-4274-B0DE-7700543ED151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E678CD98-7603-4F8D-A196-0325C6093512}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{E678CD98-7603-4F8D-A196-0325C6093512}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ESP</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>សីតុណ្ហភាព៖ សំដៅលើមាតិកាកំដៅជាក់លាក់នៃខ្យល់នៅកន្លែង និងពេលវេលាដែលបានកំណត់។ (កម្ពុជា ២១-៣៨°C)។</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Appliance charge level</t>
+  </si>
+  <si>
+    <t>Nivel de carga de los aparatos</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0E22F1-F37C-4EE3-AC5C-F090C1E074BA}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +498,7 @@
     <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -514,8 +523,11 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -540,8 +552,11 @@
       <c r="H2" t="s">
         <v>24</v>
       </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -566,8 +581,11 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -578,7 +596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Última versión del proyecto :tada:
</commit_message>
<xml_diff>
--- a/explicaciones.xlsx
+++ b/explicaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaba\Documents\Ciencia_de_Datos\Ciencia_Datos_IV\Practicas_Externas\Proyecto_Shiny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaba\Documents\Ciencia_de_Datos\Ciencia_Datos_IV\Practicas_Externas\Proyecto_Shiny\Proyecto_Wurth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792C34A5-2BA0-4274-B0DE-7700543ED151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E157B5-B63A-4E8A-AFD8-F5980194D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{E678CD98-7603-4F8D-A196-0325C6093512}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E678CD98-7603-4F8D-A196-0325C6093512}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ESP</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Idioma</t>
   </si>
   <si>
-    <t>humedad camboya</t>
-  </si>
-  <si>
     <t>Temperature: Refers to the specific heat content of the air at a given place and time.  (Cambodia 21 - 38°C).</t>
   </si>
   <si>
@@ -125,6 +122,27 @@
   </si>
   <si>
     <t>Nivel de carga de los aparatos</t>
+  </si>
+  <si>
+    <t>សំណើម៖ វាគឺជាសមាមាត្រនៃសម្ពាធផ្នែកនៃចំហាយទឹកទៅនឹងសម្ពាធចំហាយទឹកដែលមានលំនឹងនៅសីតុណ្ហភាពដែលបានផ្តល់ឱ្យ។ ដើម្បីសម្រេចបាននូវសីតុណ្ហភាពល្អបំផុតនៅក្នុងផ្ទះ វាជាការសំខាន់ណាស់ដែលសំណើមដែលទាក់ទងនៃខ្យល់គឺលើសពី 40% ហើយវាមិនលើសពី 60% ទេ។ សមាមាត្រខ្ពស់នៃសំណើមក៏ជួយដល់ការវិវត្តនៃរោគផ្លូវដង្ហើម និងការបង្កើតផ្សិតផងដែរ។</t>
+  </si>
+  <si>
+    <t>CO2៖ កាបូនឌីអុកស៊ីតគឺជាឧស្ម័នគ្មានក្លិន គ្មានពណ៌ គ្មានជាតិអាស៊ីតបន្តិច និងមិនងាយឆេះ។ ការស្រូបចូលដែលមានកំហាប់ខ្ពស់អាចបណ្តាលឱ្យមានខ្យល់ចេញចូលខ្លាំង បាត់បង់ស្មារតី tachycardia និងឈឺក្បាល។ ប្រសិនបើ​ការ​ប៉ះពាល់​យូរ​ទៅ វា​អាច​បង្ក​ឱ្យ​មាន​ការ​ប្រែប្រួល​ក្នុង​ការ​រំលាយ​អាហារ​របស់​មនុស្ស​។</t>
+  </si>
+  <si>
+    <t>CO: កាបូនម៉ូណូអុកស៊ីតគឺជាឧស្ម័នគ្មានក្លិន គ្មានពណ៌ គ្មានរសជាតិ គ្មានជាតិពុល និងងាយឆេះ បើទោះបីជាវាមិនមែនជាសារធាតុដែលឆាប់ខឹងក៏ដោយ ដូច្នេះការប៉ះពាល់អាចត្រូវបានគេកត់សម្គាល់ទាំងស្រុង។ អាចនាំអោយមានការច្របូកច្របល់ផ្លូវចិត្ត វិលមុខ ឈឺក្បាល ចង្អោរ ខ្សោយ និងបាត់បង់ស្មារតី។ ប្រសិនបើការប៉ះពាល់យូរកើតឡើង ប្រព័ន្ធប្រសាទ និងសរសៃឈាមបេះដូងអាចនឹងរងផលប៉ះពាល់ ដែលនាំឱ្យមានបញ្ហាប្រព័ន្ធប្រសាទ និងបេះដូង។</t>
+  </si>
+  <si>
+    <t>PM 1.0: ពួកវាជាភាគល្អិតព្យួរដែលមានអង្កត់ផ្ចិតខ្យល់រហូតដល់ 0.1 µm ដែលហៅថាភាគល្អិតជ្រុល ឬប្រភាគ ultrafine ។ ពួកវាមាននៅក្នុងស៊ុលហ្វាត កាបូនធាតុ សមាសធាតុលោហធាតុ និងសមាសធាតុសរីរាង្គដែលមានសម្ពាធចំហាយទឹកទាប។</t>
+  </si>
+  <si>
+    <t>PM 2.5: ពួកវាជាភាគល្អិតព្យួរដែលមានអង្កត់ផ្ចិតខ្យល់រហូតដល់ 2.5 µm ហៅថា ភាគល្អិតល្អ ឬប្រភាគល្អ។ ពួកវាជាប់ពាក់ព័ន្ធក្នុងការកើនឡើងនៃការស្លាប់ និងជំងឺដោយសារមូលហេតុផ្លូវដង្ហើម និងសរសៃឈាមបេះដូង។</t>
+  </si>
+  <si>
+    <t>PM 10: ពួកវាអាចកំណត់បានថាជាភាគល្អិតរឹង ឬរាវនៃធូលី ផេះ កំបោរ ភាគល្អិតលោហធាតុ ស៊ីម៉ងត៍ ឬលំអងដែលបែកខ្ចាត់ខ្ចាយក្នុងបរិយាកាស ហើយអង្កត់ផ្ចិតរបស់វាប្រែប្រួលចន្លោះពី 2.5 ទៅ 10 µm ។ វាអាចបណ្តាលឱ្យមានផលប៉ះពាល់ដល់ប្រព័ន្ធផ្លូវដង្ហើមរបស់មនុស្ស ប៉ុន្តែពួកវាមានះថាក់តិចជាង PM2.5 ចាប់តាំងពីមានទំហំធំជាង ពួកវាមិនអាចឆ្លងកាត់ alveoli សួតបានទេ។</t>
+  </si>
+  <si>
+    <t>កម្រិតបន្ទុកឧបករណ៍</t>
   </si>
 </sst>
 </file>
@@ -489,7 +507,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +542,7 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -532,57 +550,57 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -590,10 +608,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>